<commit_message>
First Edition Final ReadMe.
</commit_message>
<xml_diff>
--- a/result_showcase/Result Comparasion.xlsx
+++ b/result_showcase/Result Comparasion.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
     <t>BlockSize</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>Efficient Scan</t>
-  </si>
-  <si>
-    <t>Thrust Sort</t>
   </si>
   <si>
     <t xml:space="preserve">CPU Scan </t>
@@ -48,6 +45,33 @@
   </si>
   <si>
     <t>Non- Power of two</t>
+  </si>
+  <si>
+    <t>ArraySize</t>
+  </si>
+  <si>
+    <t>CPU Scan</t>
+  </si>
+  <si>
+    <t>std::sort</t>
+  </si>
+  <si>
+    <t>2^8</t>
+  </si>
+  <si>
+    <t>2^12</t>
+  </si>
+  <si>
+    <t>2^16</t>
+  </si>
+  <si>
+    <t>2^20</t>
+  </si>
+  <si>
+    <t>2^24</t>
+  </si>
+  <si>
+    <t>Thrust Scan</t>
   </si>
 </sst>
 </file>
@@ -141,7 +165,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Scan and Thrust Sort</a:t>
+              <a:t> Scan and Thrust Scan</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -381,7 +405,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Thrust Sort</c:v>
+                  <c:v>Thrust Scan</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -856,16 +880,13 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
@@ -1398,6 +1419,1499 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Compare</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Between Naive Scan, Efficient Scan, Thrust Scan, and CPU Scan</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Block Size = 128 </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Naïve Scan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$43:$A$47</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2^8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2^12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2^16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2^20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2^24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$43:$B$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.1904000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.7008000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13167999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2978240000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.539680000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-90BF-4508-945B-602CAC010DBF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Efficient Scan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-90BF-4508-945B-602CAC010DBF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$43:$A$47</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2^8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2^12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2^16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2^20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2^24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$43:$C$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.11024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14172799999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.347968</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6814720000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.6632</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-90BF-4508-945B-602CAC010DBF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Thrust Scan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$43:$A$47</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2^8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2^12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2^16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2^20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2^24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$43:$D$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.1248E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7616000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.245728</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46860800000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.403232</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-90BF-4508-945B-602CAC010DBF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPU Scan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$43:$A$47</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2^8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2^12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2^16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2^20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2^24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$43:$E$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.50129999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5041</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.0931</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-90BF-4508-945B-602CAC010DBF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1640642304"/>
+        <c:axId val="1640650624"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1640642304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1"/>
+                  <a:t>Array</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1" baseline="0"/>
+                  <a:t> Size</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.47656185908412801"/>
+              <c:y val="0.89058747471900757"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1640650624"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1640650624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Time(ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.4289485921476452E-2"/>
+              <c:y val="0.34667619803172312"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1640642304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Compare Between Radix Sort and Std::Sort</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Block Size = 128</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Radix Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$H$43:$H$47</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2^8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2^12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2^16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2^20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2^24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$43:$F$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.1053440000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2231359999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.3580480000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42.627296000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>749.64984100000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-28F7-4215-8361-F96814DCCF19}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>std::sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$H$43:$H$47</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2^8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2^12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2^16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2^20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2^24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$43:$G$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0105000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58.186799999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>894.42470000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-28F7-4215-8361-F96814DCCF19}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1570134208"/>
+        <c:axId val="1570135040"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1570134208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:t>Array</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+                  <a:t> S</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" baseline="0"/>
+                  <a:t>ize</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.47121057374255648"/>
+              <c:y val="0.89849471993258367"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1570135040"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1570135040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1"/>
+                  <a:t>Time(ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1570134208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.39270438454946227"/>
+          <c:y val="0.94453708336625142"/>
+          <c:w val="0.24260611187643452"/>
+          <c:h val="3.7625681405208972E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1478,6 +2992,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2467,6 +4061,1038 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2556,6 +5182,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>904874</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>928687</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2861,10 +5547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2873,16 +5559,23 @@
     <col min="2" max="2" width="14.875" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
     <col min="5" max="5" width="16.875" customWidth="1"/>
+    <col min="6" max="6" width="12.25" customWidth="1"/>
     <col min="7" max="7" width="26.125" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="12.375" customWidth="1"/>
+    <col min="10" max="10" width="14.625" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="12.5" customWidth="1"/>
+    <col min="13" max="13" width="17.125" customWidth="1"/>
+    <col min="14" max="14" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2896,13 +5589,13 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -2914,13 +5607,13 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
         <v>3</v>
-      </c>
-      <c r="K2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3187,6 +5880,278 @@
       </c>
       <c r="L9">
         <v>42.600200000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="H41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H42" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" t="s">
+        <v>1</v>
+      </c>
+      <c r="J42" t="s">
+        <v>2</v>
+      </c>
+      <c r="K42" t="s">
+        <v>15</v>
+      </c>
+      <c r="L42" t="s">
+        <v>8</v>
+      </c>
+      <c r="M42" t="s">
+        <v>4</v>
+      </c>
+      <c r="N42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43">
+        <v>3.1904000000000002E-2</v>
+      </c>
+      <c r="C43">
+        <v>0.11024</v>
+      </c>
+      <c r="D43">
+        <v>2.1248E-2</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>1.1053440000000001</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43">
+        <v>3.0528E-2</v>
+      </c>
+      <c r="J43">
+        <v>0.10176</v>
+      </c>
+      <c r="K43">
+        <v>1.264E-2</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>1.097664</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44">
+        <v>4.7008000000000001E-2</v>
+      </c>
+      <c r="C44">
+        <v>0.14172799999999999</v>
+      </c>
+      <c r="D44">
+        <v>2.7616000000000002E-2</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>2.2231359999999998</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44" t="s">
+        <v>11</v>
+      </c>
+      <c r="I44">
+        <v>4.5471999999999999E-2</v>
+      </c>
+      <c r="J44">
+        <v>0.167264</v>
+      </c>
+      <c r="K44">
+        <v>1.9008000000000001E-2</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>2.448928</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45">
+        <v>0.13167999999999999</v>
+      </c>
+      <c r="C45">
+        <v>0.347968</v>
+      </c>
+      <c r="D45">
+        <v>0.245728</v>
+      </c>
+      <c r="E45">
+        <v>0.50129999999999997</v>
+      </c>
+      <c r="F45">
+        <v>7.3580480000000001</v>
+      </c>
+      <c r="G45">
+        <v>4.0105000000000004</v>
+      </c>
+      <c r="H45" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45">
+        <v>0.12992000000000001</v>
+      </c>
+      <c r="J45">
+        <v>0.34467199999999998</v>
+      </c>
+      <c r="K45">
+        <v>0.21491199999999999</v>
+      </c>
+      <c r="L45">
+        <v>0.50280000000000002</v>
+      </c>
+      <c r="M45">
+        <v>7.425376</v>
+      </c>
+      <c r="N45">
+        <v>3.5099</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46">
+        <v>1.2978240000000001</v>
+      </c>
+      <c r="C46">
+        <v>1.6814720000000001</v>
+      </c>
+      <c r="D46">
+        <v>0.46860800000000002</v>
+      </c>
+      <c r="E46">
+        <v>1.5041</v>
+      </c>
+      <c r="F46">
+        <v>42.627296000000001</v>
+      </c>
+      <c r="G46">
+        <v>58.186799999999998</v>
+      </c>
+      <c r="H46" t="s">
+        <v>13</v>
+      </c>
+      <c r="I46">
+        <v>1.2931839999999999</v>
+      </c>
+      <c r="J46">
+        <v>1.6867840000000001</v>
+      </c>
+      <c r="K46">
+        <v>0.336704</v>
+      </c>
+      <c r="L46">
+        <v>1.5035000000000001</v>
+      </c>
+      <c r="M46">
+        <v>42.236992000000001</v>
+      </c>
+      <c r="N46">
+        <v>57.672800000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47">
+        <v>25.539680000000001</v>
+      </c>
+      <c r="C47">
+        <v>27.6632</v>
+      </c>
+      <c r="D47">
+        <v>2.403232</v>
+      </c>
+      <c r="E47">
+        <v>25.0931</v>
+      </c>
+      <c r="F47">
+        <v>749.64984100000004</v>
+      </c>
+      <c r="G47">
+        <v>894.42470000000003</v>
+      </c>
+      <c r="H47" t="s">
+        <v>14</v>
+      </c>
+      <c r="I47">
+        <v>25.601631000000001</v>
+      </c>
+      <c r="J47">
+        <v>25.619167000000001</v>
+      </c>
+      <c r="K47">
+        <v>2.1326399999999999</v>
+      </c>
+      <c r="L47">
+        <v>43.115699999999997</v>
+      </c>
+      <c r="M47">
+        <v>747.37829599999998</v>
+      </c>
+      <c r="N47">
+        <v>909.44740000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ReadMe Minor Mistakes Correction
</commit_message>
<xml_diff>
--- a/result_showcase/Result Comparasion.xlsx
+++ b/result_showcase/Result Comparasion.xlsx
@@ -5549,8 +5549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>